<commit_message>
modified upload file feature
</commit_message>
<xml_diff>
--- a/project/EleConsumption.xlsx
+++ b/project/EleConsumption.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21652\Documents\Projects\Energy-Management-Live-Dashboard\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alaed\Energymanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF66582C-E6F9-4452-9285-15C3129F9908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EB4CD3-A63A-40AF-950B-C74370320250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5" xr2:uid="{69947EFB-DC37-4D21-8796-D405335F5802}"/>
+    <workbookView minimized="1" xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="8" xr2:uid="{69947EFB-DC37-4D21-8796-D405335F5802}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -24,26 +24,17 @@
     <sheet name="RegThird" sheetId="10" r:id="rId9"/>
     <sheet name="Feuil5" sheetId="11" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="47">
   <si>
     <t>consumption</t>
   </si>
@@ -156,13 +147,34 @@
     <t>cost(674)</t>
   </si>
   <si>
-    <t>HDD 18</t>
-  </si>
-  <si>
-    <t>HDD 18(667)</t>
-  </si>
-  <si>
-    <t>HDD 18(666)</t>
+    <t>CDD 18(667)</t>
+  </si>
+  <si>
+    <t>CDD 18(666)</t>
+  </si>
+  <si>
+    <t>CDD25(670)</t>
+  </si>
+  <si>
+    <t>CDD25(669)</t>
+  </si>
+  <si>
+    <t>CDD25(659)</t>
+  </si>
+  <si>
+    <t>CDD25(658)</t>
+  </si>
+  <si>
+    <t>CDD25(672)</t>
+  </si>
+  <si>
+    <t>CDD25(671)</t>
+  </si>
+  <si>
+    <t>CDD25(673)</t>
+  </si>
+  <si>
+    <t>CDD25(674)</t>
   </si>
 </sst>
 </file>
@@ -170,9 +182,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_([$TND]\ * #,##0.00_);_([$TND]\ * \(#,##0.00\);_([$TND]\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_([$TND]\ * #,##0.00_);_([$TND]\ * \(#,##0.00\);_([$TND]\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -337,13 +349,13 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -370,22 +382,25 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Milliers" xfId="1" builtinId="3"/>
+    <cellStyle name="Monétaire" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -402,7 +417,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -704,7 +719,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="31.6640625" customWidth="1"/>
@@ -865,7 +880,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -879,7 +894,7 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
@@ -1216,7 +1231,7 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.5546875" customWidth="1"/>
     <col min="3" max="3" width="11.5546875" customWidth="1"/>
@@ -1631,7 +1646,7 @@
       <selection sqref="A1:A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16.44140625" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
@@ -1879,7 +1894,7 @@
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" customWidth="1"/>
@@ -2121,101 +2136,90 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F4BD80-D933-4537-93CF-2F91DE62C108}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
-        <v>133.1</v>
-      </c>
-      <c r="B2" s="9">
-        <v>3498</v>
+        <v>3.6</v>
+      </c>
+      <c r="B2" s="8">
+        <f>6948/2.25</f>
+        <v>3088</v>
       </c>
       <c r="C2" s="6">
-        <v>215</v>
-      </c>
-      <c r="D2" s="9">
-        <v>559</v>
-      </c>
-      <c r="E2" s="6">
-        <v>133.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3.6</v>
+      </c>
+      <c r="D2" s="12">
+        <f>719/2.25</f>
+        <v>319.55555555555554</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
-        <v>215</v>
-      </c>
-      <c r="B3" s="7">
-        <v>4338</v>
+        <v>65.099999999999994</v>
+      </c>
+      <c r="B3" s="8">
+        <f>6948/1.8</f>
+        <v>3860</v>
       </c>
       <c r="C3" s="6">
-        <v>170.4</v>
-      </c>
-      <c r="D3" s="7">
-        <v>448</v>
-      </c>
-      <c r="E3" s="6">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="D3" s="12">
+        <f>719/1.8</f>
+        <v>399.44444444444446</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
-        <v>170.4</v>
+        <v>132</v>
       </c>
       <c r="B4" s="7">
-        <v>4677</v>
+        <v>4038</v>
       </c>
       <c r="C4" s="6">
-        <v>67.3</v>
-      </c>
-      <c r="D4" s="7">
-        <v>361</v>
-      </c>
-      <c r="E4" s="6">
-        <v>170.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+      <c r="D4" s="12">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
-        <v>118.7</v>
+        <v>136.4</v>
       </c>
       <c r="B5" s="7">
-        <v>3101</v>
+        <v>4612</v>
       </c>
       <c r="C5" s="6">
-        <v>34.799999999999997</v>
-      </c>
-      <c r="D5" s="36">
-        <v>320</v>
-      </c>
-      <c r="E5" s="6">
-        <v>118.7</v>
+        <v>136.4</v>
+      </c>
+      <c r="D5" s="11">
+        <v>983</v>
       </c>
     </row>
   </sheetData>
@@ -2225,56 +2229,358 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E915918-0B56-4C6B-AAFC-E402EDE81EBB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="36">
+        <v>3.6</v>
+      </c>
+      <c r="B2" s="8">
+        <f>10464/2.25</f>
+        <v>4650.666666666667</v>
+      </c>
+      <c r="C2" s="6">
+        <v>3.6</v>
+      </c>
+      <c r="D2" s="12">
+        <f>2422/2.25</f>
+        <v>1076.4444444444443</v>
+      </c>
+      <c r="E2" s="6">
+        <v>3.6</v>
+      </c>
+      <c r="F2" s="12">
+        <f>2596/2.25</f>
+        <v>1153.7777777777778</v>
+      </c>
+      <c r="G2" s="6">
+        <v>3.6</v>
+      </c>
+      <c r="H2" s="12">
+        <f>3140/2.25</f>
+        <v>1395.5555555555557</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="36">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="B3" s="8">
+        <f>10464/1.8</f>
+        <v>5813.333333333333</v>
+      </c>
+      <c r="C3" s="6">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="D3" s="12">
+        <f>2422/1.8</f>
+        <v>1345.5555555555554</v>
+      </c>
+      <c r="E3" s="6">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="F3" s="12">
+        <f>2596/1.8</f>
+        <v>1442.2222222222222</v>
+      </c>
+      <c r="G3" s="6">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="H3" s="12">
+        <f>3140/1.8</f>
+        <v>1744.4444444444443</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="36">
+        <v>132</v>
+      </c>
+      <c r="B4" s="7">
+        <v>6562</v>
+      </c>
+      <c r="C4" s="6">
+        <v>132</v>
+      </c>
+      <c r="D4" s="14">
+        <v>1309</v>
+      </c>
+      <c r="E4" s="6">
+        <v>132</v>
+      </c>
+      <c r="F4" s="14">
+        <v>2876</v>
+      </c>
+      <c r="G4" s="6">
+        <v>132</v>
+      </c>
+      <c r="H4" s="19">
+        <v>2914</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="36">
+        <v>136.4</v>
+      </c>
+      <c r="B5" s="8">
+        <v>7240</v>
+      </c>
+      <c r="C5" s="6">
+        <v>136.4</v>
+      </c>
+      <c r="D5" s="14">
+        <v>1731</v>
+      </c>
+      <c r="E5" s="6">
+        <v>136.4</v>
+      </c>
+      <c r="F5" s="14">
+        <v>2633</v>
+      </c>
+      <c r="G5" s="6">
+        <v>136.4</v>
+      </c>
+      <c r="H5" s="19">
+        <v>2818</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7515690-C4FA-4B07-8896-918B36B84B5C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.21875" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>3.6</v>
+      </c>
+      <c r="B2" s="12">
+        <f>3328/2.25</f>
+        <v>1479.1111111111111</v>
+      </c>
+      <c r="C2" s="6">
+        <v>3.6</v>
+      </c>
+      <c r="D2" s="12">
+        <f>1582/2.25</f>
+        <v>703.11111111111109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="B3" s="12">
+        <f>3328/1.8</f>
+        <v>1848.8888888888889</v>
+      </c>
+      <c r="C3" s="6">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="D3" s="12">
+        <f>1582/1.8</f>
+        <v>878.88888888888891</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>132</v>
+      </c>
+      <c r="B4" s="12">
+        <v>3015</v>
+      </c>
+      <c r="C4" s="6">
+        <v>132</v>
+      </c>
+      <c r="D4" s="12">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>136.4</v>
+      </c>
+      <c r="B5" s="14">
+        <v>2927</v>
+      </c>
+      <c r="C5" s="6">
+        <v>136.4</v>
+      </c>
+      <c r="D5" s="12">
+        <v>1310</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34FED05-A64E-403A-B5AF-E9F0914CA14A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>3.6</v>
+      </c>
+      <c r="B2" s="12">
+        <f>1876/2.25</f>
+        <v>833.77777777777783</v>
+      </c>
+      <c r="C2" s="37">
+        <v>3.6</v>
+      </c>
+      <c r="D2" s="12">
+        <f>1920/2.25</f>
+        <v>853.33333333333337</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="B3" s="12">
+        <f>1876/1.8</f>
+        <v>1042.2222222222222</v>
+      </c>
+      <c r="C3" s="37">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="D3" s="12">
+        <f>1920/1.8</f>
+        <v>1066.6666666666667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>132</v>
+      </c>
+      <c r="B4" s="14">
+        <v>1876</v>
+      </c>
+      <c r="C4" s="37">
+        <v>132</v>
+      </c>
+      <c r="D4" s="24">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>136.4</v>
+      </c>
+      <c r="B5" s="14">
+        <v>1313</v>
+      </c>
+      <c r="C5" s="37">
+        <v>136.4</v>
+      </c>
+      <c r="D5" s="24">
+        <v>2103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>47</v>
+      </c>
+      <c r="B6" s="23">
+        <v>1548</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000207857AF682EB4296FCF42D4E0EAFCD" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="20477786a0ad41f446667ecb934996bd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f50bce7f-2e55-4283-ad3f-2d53e508549c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c0ee13160c64bd76dddc95fe7ca5f7f8" ns2:_="">
     <xsd:import namespace="f50bce7f-2e55-4283-ad3f-2d53e508549c"/>
@@ -2406,24 +2712,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24037C15-6C58-4C98-87B4-814001D7D068}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1030D94-C29C-4CF5-8137-89C2463ABCEE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2142E4E7-6E49-4E12-9E63-C43BA88CD15B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2439,4 +2743,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1030D94-C29C-4CF5-8137-89C2463ABCEE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24037C15-6C58-4C98-87B4-814001D7D068}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>